<commit_message>
adapted tests for new olink format
</commit_message>
<xml_diff>
--- a/tests/services/data/olink_data.xlsx
+++ b/tests/services/data/olink_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-api-gae/tests/services/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E36A0D-5833-224F-8FC4-88A2D601632A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7B5895-54E7-3F44-818E-C269310E40E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7340" yWindow="960" windowWidth="20300" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{13EB5F58-6F5B-0C43-B3A3-FDD559CF4102}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{617EE495-57B5-7A45-B78B-2BA5C7270B47}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chip barcode number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{13EB5F58-6F5B-0C43-B3A3-FDD559CF4102}">
       <text>
         <r>
           <rPr>
@@ -64,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{4DC57F73-054D-6848-9835-CD754B758745}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{4DC57F73-054D-6848-9835-CD754B758745}">
       <text>
         <r>
           <rPr>
@@ -77,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{6F24E415-9A94-2A40-920E-6B70436A6172}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{6F24E415-9A94-2A40-920E-6B70436A6172}">
       <text>
         <r>
           <rPr>
@@ -90,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{11306FA7-522C-4B42-95A7-66DB719B8B0A}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{11306FA7-522C-4B42-95A7-66DB719B8B0A}">
       <text>
         <r>
           <rPr>
@@ -103,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{973DD079-B71E-F34B-A08C-9C72391A5A36}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{973DD079-B71E-F34B-A08C-9C72391A5A36}">
       <text>
         <r>
           <rPr>
@@ -116,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{26E4C8BE-C185-074D-97D6-9576E910C5F4}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{26E4C8BE-C185-074D-97D6-9576E910C5F4}">
       <text>
         <r>
           <rPr>
@@ -129,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{BC135B00-8EB0-A447-9007-86B1984491AC}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{BC135B00-8EB0-A447-9007-86B1984491AC}">
       <text>
         <r>
           <rPr>
@@ -139,19 +152,6 @@
             <family val="2"/>
           </rPr>
           <t>Build of the Fluidgm application used</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{617EE495-57B5-7A45-B78B-2BA5C7270B47}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chip barcode number</t>
         </r>
       </text>
     </comment>
@@ -880,7 +880,7 @@
   <dimension ref="A1:Q210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1087,28 +1087,28 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>18</v>
@@ -1137,29 +1137,29 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11">
+        <v>111</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>43811</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>26</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>27</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>20140305.43</v>
-      </c>
-      <c r="I11">
-        <v>13456777</v>
       </c>
       <c r="J11" t="s">
         <v>28</v>
@@ -1187,29 +1187,29 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12">
+        <v>112</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>43811</v>
       </c>
-      <c r="E12" s="5">
+      <c r="F12" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>26</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>27</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>20140305.43</v>
-      </c>
-      <c r="I12">
-        <v>13456777</v>
       </c>
       <c r="J12" t="s">
         <v>28</v>
@@ -2232,12 +2232,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{71FCE423-CB7D-684A-BC25-3FB6CBA1578C}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="E11:E12" xr:uid="{BDEFDE59-F742-9C43-AFAB-0BF15DCB45FF}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="F11:F12" xr:uid="{BDEFDE59-F742-9C43-AFAB-0BF15DCB45FF}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D11:D12" xr:uid="{AD9CD908-0D70-114B-8B87-FE6338128C34}">
-      <formula1>AND(ISNUMBER(D11:D210),LEFT(CELL("format",D11:D210),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E11:E12" xr:uid="{AD9CD908-0D70-114B-8B87-FE6338128C34}">
+      <formula1>AND(ISNUMBER(D14:D210),LEFT(CELL("format",D14:D210),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>